<commit_message>
Add More Mock Credentials
</commit_message>
<xml_diff>
--- a/TestRunner/Data/CREDENTIALS.XLSX
+++ b/TestRunner/Data/CREDENTIALS.XLSX
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C4E1CE-8042-4B1C-8210-DC070D909BE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221E6A50-9273-431A-AC3F-273A05014143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16485" yWindow="3705" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATASET" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>USERNAME</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>localhost@microsoft.com</t>
+  </si>
+  <si>
+    <t>root@ubuntu.org</t>
+  </si>
+  <si>
+    <t>admin@stackworks.online</t>
+  </si>
+  <si>
+    <t>syspass</t>
+  </si>
+  <si>
+    <t>sudologin</t>
+  </si>
+  <si>
+    <t>letmein</t>
   </si>
 </sst>
 </file>
@@ -67,8 +79,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,35 +367,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix "No Data Is Available For Encoding 1252" Error
</commit_message>
<xml_diff>
--- a/TestRunner/Data/CREDENTIALS.XLSX
+++ b/TestRunner/Data/CREDENTIALS.XLSX
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221E6A50-9273-431A-AC3F-273A05014143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VLOOD\Source\Repos\Z34-Test-Automation-Framework\TestRunner\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72279AA0-AED0-41A1-A3B1-027D2869A969}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16485" yWindow="3705" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATASET" sheetId="1" r:id="rId1"/>
@@ -22,25 +27,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
     <t>localhost@microsoft.com</t>
   </si>
   <si>
+    <t>syspass</t>
+  </si>
+  <si>
     <t>root@ubuntu.org</t>
   </si>
   <si>
+    <t>sudologin</t>
+  </si>
+  <si>
     <t>admin@stackworks.online</t>
-  </si>
-  <si>
-    <t>syspass</t>
-  </si>
-  <si>
-    <t>sudologin</t>
   </si>
   <si>
     <t>letmein</t>
@@ -79,14 +84,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,50 +369,48 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>